<commit_message>
updated DEAN import format
</commit_message>
<xml_diff>
--- a/DEAN_import_format.xlsx
+++ b/DEAN_import_format.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Person" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t xml:space="preserve">person_id</t>
   </si>
@@ -89,6 +89,36 @@
   </si>
   <si>
     <t xml:space="preserve">enrollment_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enrollment_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">completion_flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">completion_success_flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">withdrawal_flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drop_flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enrollment_status_change_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">course_grade_final_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">course_grade_final_letter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">course_grade_to_date_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">course_grade_to_date_letter</t>
   </si>
 </sst>
 </file>
@@ -218,7 +248,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -324,8 +354,8 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -394,17 +424,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0333333333333"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.562962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.2481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9481481481481"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.0111111111111"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7444444444444"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.6555555555556"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.5333333333333"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.5111111111111"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.1518518518519"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.1333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -413,6 +454,39 @@
       </c>
       <c r="B1" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>